<commit_message>
rev -- add missing indicator target
</commit_message>
<xml_diff>
--- a/data-raw/unhcr_2020/iati_document_link.xlsx
+++ b/data-raw/unhcr_2020/iati_document_link.xlsx
@@ -439,7 +439,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">http://innovation.unhcr.org  </t>
+          <t>http://innovation.unhcr.org  </t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -21418,7 +21418,7 @@
       </c>
       <c r="B570" t="inlineStr">
         <is>
-          <t xml:space="preserve">http://innovation.unhcr.org  </t>
+          <t>http://innovation.unhcr.org  </t>
         </is>
       </c>
       <c r="C570" t="inlineStr">

</xml_diff>